<commit_message>
26.11.2020 MC Sales Detils
</commit_message>
<xml_diff>
--- a/2020/November/All Details/24.11.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/November/All Details/24.11.2020/MC Bank Statement Sep-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 2020" sheetId="7" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="219">
   <si>
     <t>Date</t>
   </si>
@@ -781,25 +781,16 @@
     <t>Jamil Bhaira</t>
   </si>
   <si>
-    <t>Mokul Tel</t>
-  </si>
-  <si>
     <t>23.11.2020</t>
-  </si>
-  <si>
-    <t>Date: 23.11.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hasan </t>
-  </si>
-  <si>
-    <t>Galaxy</t>
   </si>
   <si>
     <t>DSR Herok</t>
   </si>
   <si>
     <t>24.11.2020</t>
+  </si>
+  <si>
+    <t>Date: 24.11.2020</t>
   </si>
 </sst>
 </file>
@@ -3070,6 +3061,30 @@
     <xf numFmtId="2" fontId="39" fillId="35" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3100,34 +3115,10 @@
     <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3221,7 +3212,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3233,7 +3224,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3256,14 +3247,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3300,7 +3291,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3312,7 +3303,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3335,14 +3326,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3374,7 +3365,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3386,7 +3377,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3409,14 +3400,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3772,7 +3763,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4238,7 +4229,7 @@
     <row r="27" spans="1:8">
       <c r="A27" s="35"/>
       <c r="B27" s="40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C27" s="39">
         <v>485000</v>
@@ -4256,12 +4247,18 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="35"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
+      <c r="B28" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" s="39">
+        <v>400000</v>
+      </c>
+      <c r="D28" s="283">
+        <v>500000</v>
+      </c>
       <c r="E28" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F28" s="31"/>
       <c r="G28" s="2"/>
@@ -4274,7 +4271,7 @@
       <c r="D29" s="39"/>
       <c r="E29" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F29" s="31"/>
       <c r="G29" s="2"/>
@@ -4287,7 +4284,7 @@
       <c r="D30" s="39"/>
       <c r="E30" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="2"/>
@@ -4300,7 +4297,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="2"/>
@@ -4313,7 +4310,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F32" s="31"/>
       <c r="G32" s="2"/>
@@ -4326,7 +4323,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F33" s="31"/>
       <c r="G33" s="2"/>
@@ -4339,7 +4336,7 @@
       <c r="D34" s="39"/>
       <c r="E34" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F34" s="31"/>
       <c r="G34" s="2"/>
@@ -4352,7 +4349,7 @@
       <c r="D35" s="39"/>
       <c r="E35" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F35" s="31"/>
       <c r="G35" s="2"/>
@@ -4365,7 +4362,7 @@
       <c r="D36" s="39"/>
       <c r="E36" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F36" s="31"/>
       <c r="G36" s="2"/>
@@ -4378,7 +4375,7 @@
       <c r="D37" s="39"/>
       <c r="E37" s="41">
         <f t="shared" si="0"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F37" s="31"/>
       <c r="G37" s="2"/>
@@ -4391,7 +4388,7 @@
       <c r="D38" s="39"/>
       <c r="E38" s="41">
         <f t="shared" ref="E38:E69" si="1">E37+C38-D38</f>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F38" s="31"/>
       <c r="G38" s="2"/>
@@ -4404,7 +4401,7 @@
       <c r="D39" s="39"/>
       <c r="E39" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F39" s="31"/>
       <c r="G39" s="2"/>
@@ -4417,7 +4414,7 @@
       <c r="D40" s="39"/>
       <c r="E40" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F40" s="31"/>
       <c r="G40" s="2"/>
@@ -4430,7 +4427,7 @@
       <c r="D41" s="39"/>
       <c r="E41" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F41" s="31"/>
       <c r="G41" s="2"/>
@@ -4443,7 +4440,7 @@
       <c r="D42" s="39"/>
       <c r="E42" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F42" s="31"/>
       <c r="G42" s="2"/>
@@ -4456,7 +4453,7 @@
       <c r="D43" s="39"/>
       <c r="E43" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F43" s="31"/>
       <c r="G43" s="2"/>
@@ -4469,7 +4466,7 @@
       <c r="D44" s="39"/>
       <c r="E44" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F44" s="31"/>
       <c r="G44" s="2"/>
@@ -4482,7 +4479,7 @@
       <c r="D45" s="39"/>
       <c r="E45" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F45" s="31"/>
       <c r="G45" s="2"/>
@@ -4495,7 +4492,7 @@
       <c r="D46" s="39"/>
       <c r="E46" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F46" s="31"/>
       <c r="G46" s="2"/>
@@ -4508,7 +4505,7 @@
       <c r="D47" s="39"/>
       <c r="E47" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F47" s="31"/>
       <c r="G47" s="2"/>
@@ -4521,7 +4518,7 @@
       <c r="D48" s="39"/>
       <c r="E48" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F48" s="31"/>
       <c r="G48" s="2"/>
@@ -4533,7 +4530,7 @@
       <c r="D49" s="39"/>
       <c r="E49" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F49" s="31"/>
       <c r="G49" s="2"/>
@@ -4545,7 +4542,7 @@
       <c r="D50" s="39"/>
       <c r="E50" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F50" s="31"/>
       <c r="G50" s="2"/>
@@ -4557,7 +4554,7 @@
       <c r="D51" s="39"/>
       <c r="E51" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F51" s="31"/>
       <c r="G51" s="2"/>
@@ -4569,7 +4566,7 @@
       <c r="D52" s="39"/>
       <c r="E52" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F52" s="31"/>
       <c r="G52" s="2"/>
@@ -4581,7 +4578,7 @@
       <c r="D53" s="39"/>
       <c r="E53" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F53" s="31"/>
       <c r="G53" s="2"/>
@@ -4593,7 +4590,7 @@
       <c r="D54" s="39"/>
       <c r="E54" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F54" s="31"/>
       <c r="G54" s="2"/>
@@ -4605,7 +4602,7 @@
       <c r="D55" s="39"/>
       <c r="E55" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F55" s="31"/>
       <c r="G55" s="2"/>
@@ -4616,7 +4613,7 @@
       <c r="D56" s="39"/>
       <c r="E56" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F56" s="31"/>
       <c r="G56" s="2"/>
@@ -4627,7 +4624,7 @@
       <c r="D57" s="39"/>
       <c r="E57" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F57" s="31"/>
       <c r="G57" s="2"/>
@@ -4638,7 +4635,7 @@
       <c r="D58" s="39"/>
       <c r="E58" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F58" s="31"/>
       <c r="G58" s="2"/>
@@ -4649,7 +4646,7 @@
       <c r="D59" s="39"/>
       <c r="E59" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F59" s="31"/>
       <c r="G59" s="2"/>
@@ -4660,7 +4657,7 @@
       <c r="D60" s="39"/>
       <c r="E60" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F60" s="31"/>
       <c r="G60" s="2"/>
@@ -4671,7 +4668,7 @@
       <c r="D61" s="39"/>
       <c r="E61" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F61" s="31"/>
       <c r="G61" s="2"/>
@@ -4682,7 +4679,7 @@
       <c r="D62" s="39"/>
       <c r="E62" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F62" s="31"/>
       <c r="G62" s="2"/>
@@ -4693,7 +4690,7 @@
       <c r="D63" s="39"/>
       <c r="E63" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F63" s="31"/>
       <c r="G63" s="2"/>
@@ -4704,7 +4701,7 @@
       <c r="D64" s="39"/>
       <c r="E64" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F64" s="31"/>
       <c r="G64" s="2"/>
@@ -4715,7 +4712,7 @@
       <c r="D65" s="39"/>
       <c r="E65" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F65" s="31"/>
       <c r="G65" s="2"/>
@@ -4726,7 +4723,7 @@
       <c r="D66" s="39"/>
       <c r="E66" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F66" s="31"/>
       <c r="G66" s="2"/>
@@ -4737,7 +4734,7 @@
       <c r="D67" s="39"/>
       <c r="E67" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F67" s="31"/>
       <c r="G67" s="2"/>
@@ -4748,7 +4745,7 @@
       <c r="D68" s="39"/>
       <c r="E68" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="2"/>
@@ -4759,7 +4756,7 @@
       <c r="D69" s="39"/>
       <c r="E69" s="41">
         <f t="shared" si="1"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F69" s="31"/>
       <c r="G69" s="2"/>
@@ -4770,7 +4767,7 @@
       <c r="D70" s="39"/>
       <c r="E70" s="41">
         <f t="shared" ref="E70:E82" si="2">E69+C70-D70</f>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F70" s="31"/>
       <c r="G70" s="2"/>
@@ -4781,7 +4778,7 @@
       <c r="D71" s="39"/>
       <c r="E71" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F71" s="31"/>
       <c r="G71" s="2"/>
@@ -4792,7 +4789,7 @@
       <c r="D72" s="39"/>
       <c r="E72" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F72" s="31"/>
       <c r="G72" s="2"/>
@@ -4803,7 +4800,7 @@
       <c r="D73" s="39"/>
       <c r="E73" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F73" s="31"/>
       <c r="G73" s="2"/>
@@ -4814,7 +4811,7 @@
       <c r="D74" s="39"/>
       <c r="E74" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F74" s="31"/>
       <c r="G74" s="2"/>
@@ -4825,7 +4822,7 @@
       <c r="D75" s="39"/>
       <c r="E75" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F75" s="33"/>
       <c r="G75" s="2"/>
@@ -4836,7 +4833,7 @@
       <c r="D76" s="39"/>
       <c r="E76" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F76" s="31"/>
       <c r="G76" s="2"/>
@@ -4847,7 +4844,7 @@
       <c r="D77" s="39"/>
       <c r="E77" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F77" s="31"/>
       <c r="G77" s="2"/>
@@ -4858,7 +4855,7 @@
       <c r="D78" s="39"/>
       <c r="E78" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F78" s="31"/>
       <c r="G78" s="2"/>
@@ -4869,7 +4866,7 @@
       <c r="D79" s="39"/>
       <c r="E79" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F79" s="31"/>
       <c r="G79" s="2"/>
@@ -4880,7 +4877,7 @@
       <c r="D80" s="39"/>
       <c r="E80" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F80" s="31"/>
       <c r="G80" s="2"/>
@@ -4891,7 +4888,7 @@
       <c r="D81" s="39"/>
       <c r="E81" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F81" s="31"/>
       <c r="G81" s="2"/>
@@ -4902,7 +4899,7 @@
       <c r="D82" s="39"/>
       <c r="E82" s="41">
         <f t="shared" si="2"/>
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F82" s="31"/>
       <c r="G82" s="2"/>
@@ -4911,15 +4908,15 @@
       <c r="B83" s="45"/>
       <c r="C83" s="41">
         <f>SUM(C5:C72)</f>
-        <v>10296844</v>
+        <v>10696844</v>
       </c>
       <c r="D83" s="41">
         <f>SUM(D5:D77)</f>
-        <v>7200000</v>
+        <v>7700000</v>
       </c>
       <c r="E83" s="66">
         <f>E71+C83-D83</f>
-        <v>6193688</v>
+        <v>5993688</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="2"/>
@@ -4947,8 +4944,8 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4978,7 +4975,7 @@
     </row>
     <row r="2" spans="1:29" ht="23.25">
       <c r="A2" s="302" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B2" s="303"/>
       <c r="C2" s="303"/>
@@ -5052,7 +5049,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="72">
-        <v>1524454.0477</v>
+        <v>1465887.2574999998</v>
       </c>
       <c r="F4" s="63"/>
       <c r="G4" s="55"/>
@@ -5084,14 +5081,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="71">
-        <v>225766.05911428534</v>
+        <v>238863.82841428538</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="68" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="72">
-        <v>3096844</v>
+        <v>2996844</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="55"/>
@@ -5124,14 +5121,14 @@
       </c>
       <c r="B6" s="71">
         <f>B4+B5</f>
-        <v>8726507.0591142848</v>
+        <v>8739604.8284142856</v>
       </c>
       <c r="C6" s="68"/>
       <c r="D6" s="68" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="282">
-        <v>495475</v>
+        <v>570614</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="55"/>
@@ -5168,7 +5165,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="73">
-        <v>2377417</v>
+        <v>2360677</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="55"/>
@@ -5200,7 +5197,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="71">
-        <v>45120</v>
+        <v>49221</v>
       </c>
       <c r="C8" s="70"/>
       <c r="D8" s="68" t="s">
@@ -5281,14 +5278,14 @@
       </c>
       <c r="B10" s="75">
         <f>B5-B8-B9</f>
-        <v>180646.05911428534</v>
+        <v>189642.82841428538</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" s="68" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="73">
-        <v>1044188.0114142848</v>
+        <v>1153352.5709142853</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>185</v>
@@ -5399,7 +5396,7 @@
       </c>
       <c r="B13" s="74">
         <f>B6-B8-B11+B12-B9</f>
-        <v>8631387.0591142848</v>
+        <v>8640383.8284142856</v>
       </c>
       <c r="C13" s="70"/>
       <c r="D13" s="70" t="s">
@@ -5407,7 +5404,7 @@
       </c>
       <c r="E13" s="73">
         <f>E4+E5+E6+E7+E8+E9+E10</f>
-        <v>8631387.0591142848</v>
+        <v>8640383.8284142856</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="283">
@@ -10665,7 +10662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
@@ -12392,7 +12389,7 @@
     </row>
     <row r="24" spans="1:61">
       <c r="A24" s="111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B24" s="112">
         <v>538735</v>
@@ -12467,13 +12464,21 @@
       <c r="BI24" s="294"/>
     </row>
     <row r="25" spans="1:61">
-      <c r="A25" s="111"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
+      <c r="A25" s="111" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="112">
+        <v>551915</v>
+      </c>
+      <c r="C25" s="112">
+        <v>564554</v>
+      </c>
+      <c r="D25" s="112">
+        <v>4101</v>
+      </c>
       <c r="E25" s="112">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>568655</v>
       </c>
       <c r="F25" s="121"/>
       <c r="G25" s="102"/>
@@ -13014,23 +13019,23 @@
       </c>
       <c r="B33" s="112">
         <f>SUM(B5:B32)</f>
-        <v>9613500</v>
+        <v>10165415</v>
       </c>
       <c r="C33" s="112">
         <f>SUM(C5:C32)</f>
-        <v>9789115</v>
+        <v>10353669</v>
       </c>
       <c r="D33" s="112">
         <f>SUM(D5:D32)</f>
-        <v>46045</v>
+        <v>50146</v>
       </c>
       <c r="E33" s="112">
         <f>SUM(E5:E32)</f>
-        <v>9835160</v>
+        <v>10403815</v>
       </c>
       <c r="F33" s="120">
         <f>B33-E33</f>
-        <v>-221660</v>
+        <v>-238400</v>
       </c>
       <c r="G33" s="134"/>
       <c r="H33" s="141"/>
@@ -13443,10 +13448,10 @@
         <v>50</v>
       </c>
       <c r="C39" s="112">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="D39" s="151" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E39" s="117"/>
       <c r="F39" s="113"/>
@@ -13588,7 +13593,7 @@
         <v>9440</v>
       </c>
       <c r="D41" s="105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E41" s="155"/>
       <c r="F41" s="113"/>
@@ -14261,10 +14266,10 @@
       </c>
       <c r="B51" s="109"/>
       <c r="C51" s="179">
-        <v>74300</v>
+        <v>74210</v>
       </c>
       <c r="D51" s="183" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E51" s="117"/>
       <c r="F51" s="109"/>
@@ -14402,7 +14407,7 @@
         <v>397451</v>
       </c>
       <c r="D53" s="186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E53" s="117"/>
       <c r="F53" s="110"/>
@@ -14471,7 +14476,7 @@
         <v>189880</v>
       </c>
       <c r="D54" s="175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E54" s="117"/>
       <c r="F54" s="295"/>
@@ -14670,16 +14675,10 @@
       <c r="BI56" s="294"/>
     </row>
     <row r="57" spans="1:61">
-      <c r="A57" s="182" t="s">
-        <v>215</v>
-      </c>
+      <c r="A57" s="182"/>
       <c r="B57" s="109"/>
-      <c r="C57" s="179">
-        <v>4000</v>
-      </c>
-      <c r="D57" s="183" t="s">
-        <v>216</v>
-      </c>
+      <c r="C57" s="179"/>
+      <c r="D57" s="183"/>
       <c r="E57" s="117"/>
       <c r="F57" s="109"/>
       <c r="G57" s="295"/>
@@ -14744,10 +14743,10 @@
       </c>
       <c r="B58" s="109"/>
       <c r="C58" s="179">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="D58" s="183" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E58" s="117"/>
       <c r="F58" s="110"/>
@@ -14873,16 +14872,10 @@
       <c r="BI59" s="294"/>
     </row>
     <row r="60" spans="1:61">
-      <c r="A60" s="182" t="s">
-        <v>219</v>
-      </c>
+      <c r="A60" s="182"/>
       <c r="B60" s="180"/>
-      <c r="C60" s="179">
-        <v>4650</v>
-      </c>
-      <c r="D60" s="180" t="s">
-        <v>216</v>
-      </c>
+      <c r="C60" s="179"/>
+      <c r="D60" s="180"/>
       <c r="E60" s="117"/>
       <c r="F60" s="109"/>
       <c r="G60" s="295"/>
@@ -15411,10 +15404,10 @@
       </c>
       <c r="B67" s="109"/>
       <c r="C67" s="179">
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="D67" s="180" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E67" s="117"/>
       <c r="F67" s="190"/>
@@ -16441,7 +16434,7 @@
         <v>15330</v>
       </c>
       <c r="D80" s="183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E80" s="117"/>
       <c r="F80" s="197"/>
@@ -16681,7 +16674,7 @@
         <v>5480</v>
       </c>
       <c r="D83" s="183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E83" s="118"/>
       <c r="F83" s="201"/>
@@ -16921,7 +16914,7 @@
         <v>3500</v>
       </c>
       <c r="D86" s="183" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E86" s="118"/>
       <c r="F86" s="197"/>
@@ -17155,16 +17148,10 @@
       <c r="BI88" s="294"/>
     </row>
     <row r="89" spans="1:61">
-      <c r="A89" s="182" t="s">
-        <v>218</v>
-      </c>
+      <c r="A89" s="182"/>
       <c r="B89" s="109"/>
-      <c r="C89" s="179">
-        <v>11000</v>
-      </c>
-      <c r="D89" s="186" t="s">
-        <v>216</v>
-      </c>
+      <c r="C89" s="179"/>
+      <c r="D89" s="186"/>
       <c r="E89" s="117"/>
       <c r="F89" s="197"/>
       <c r="G89" s="191" t="s">
@@ -17460,14 +17447,14 @@
     </row>
     <row r="93" spans="1:61">
       <c r="A93" s="182" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B93" s="180"/>
       <c r="C93" s="179">
         <v>200</v>
       </c>
       <c r="D93" s="180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F93" s="197"/>
       <c r="G93" s="195" t="s">
@@ -19037,7 +19024,7 @@
       <c r="B113" s="310"/>
       <c r="C113" s="204">
         <f>SUM(C37:C112)</f>
-        <v>2377417</v>
+        <v>2360677</v>
       </c>
       <c r="D113" s="205"/>
       <c r="F113" s="197"/>
@@ -19190,7 +19177,7 @@
       <c r="B115" s="312"/>
       <c r="C115" s="209">
         <f>C113+L136</f>
-        <v>2377417</v>
+        <v>2360677</v>
       </c>
       <c r="D115" s="210"/>
       <c r="F115" s="190"/>
@@ -21806,11 +21793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="14" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="10" ySplit="14" topLeftCell="K33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
+      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21821,94 +21808,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="331" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="323"/>
-      <c r="C1" s="323"/>
-      <c r="D1" s="323"/>
-      <c r="E1" s="323"/>
-      <c r="F1" s="323"/>
-      <c r="G1" s="323"/>
-      <c r="H1" s="323"/>
-      <c r="I1" s="323"/>
-      <c r="J1" s="323"/>
-      <c r="K1" s="323"/>
-      <c r="L1" s="323"/>
-      <c r="M1" s="323"/>
-      <c r="N1" s="323"/>
-      <c r="O1" s="323"/>
-      <c r="P1" s="323"/>
-      <c r="Q1" s="323"/>
-      <c r="R1" s="323"/>
-      <c r="S1" s="323"/>
+      <c r="B1" s="331"/>
+      <c r="C1" s="331"/>
+      <c r="D1" s="331"/>
+      <c r="E1" s="331"/>
+      <c r="F1" s="331"/>
+      <c r="G1" s="331"/>
+      <c r="H1" s="331"/>
+      <c r="I1" s="331"/>
+      <c r="J1" s="331"/>
+      <c r="K1" s="331"/>
+      <c r="L1" s="331"/>
+      <c r="M1" s="331"/>
+      <c r="N1" s="331"/>
+      <c r="O1" s="331"/>
+      <c r="P1" s="331"/>
+      <c r="Q1" s="331"/>
+      <c r="R1" s="331"/>
+      <c r="S1" s="331"/>
     </row>
     <row r="2" spans="1:26" s="231" customFormat="1" ht="18">
-      <c r="A2" s="324" t="s">
+      <c r="A2" s="332" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="324"/>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="324"/>
-      <c r="F2" s="324"/>
-      <c r="G2" s="324"/>
-      <c r="H2" s="324"/>
-      <c r="I2" s="324"/>
-      <c r="J2" s="324"/>
-      <c r="K2" s="324"/>
-      <c r="L2" s="324"/>
-      <c r="M2" s="324"/>
-      <c r="N2" s="324"/>
-      <c r="O2" s="324"/>
-      <c r="P2" s="324"/>
-      <c r="Q2" s="324"/>
-      <c r="R2" s="324"/>
-      <c r="S2" s="324"/>
+      <c r="B2" s="332"/>
+      <c r="C2" s="332"/>
+      <c r="D2" s="332"/>
+      <c r="E2" s="332"/>
+      <c r="F2" s="332"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
+      <c r="I2" s="332"/>
+      <c r="J2" s="332"/>
+      <c r="K2" s="332"/>
+      <c r="L2" s="332"/>
+      <c r="M2" s="332"/>
+      <c r="N2" s="332"/>
+      <c r="O2" s="332"/>
+      <c r="P2" s="332"/>
+      <c r="Q2" s="332"/>
+      <c r="R2" s="332"/>
+      <c r="S2" s="332"/>
     </row>
     <row r="3" spans="1:26" s="231" customFormat="1">
-      <c r="A3" s="325"/>
-      <c r="B3" s="325"/>
-      <c r="C3" s="325"/>
-      <c r="D3" s="325"/>
-      <c r="E3" s="325"/>
-      <c r="F3" s="325"/>
-      <c r="G3" s="325"/>
-      <c r="H3" s="325"/>
-      <c r="I3" s="325"/>
-      <c r="J3" s="325"/>
-      <c r="K3" s="325"/>
-      <c r="L3" s="325"/>
-      <c r="M3" s="325"/>
-      <c r="N3" s="325"/>
-      <c r="O3" s="325"/>
-      <c r="P3" s="325"/>
-      <c r="Q3" s="325"/>
-      <c r="R3" s="325"/>
-      <c r="S3" s="325"/>
+      <c r="A3" s="333"/>
+      <c r="B3" s="333"/>
+      <c r="C3" s="333"/>
+      <c r="D3" s="333"/>
+      <c r="E3" s="333"/>
+      <c r="F3" s="333"/>
+      <c r="G3" s="333"/>
+      <c r="H3" s="333"/>
+      <c r="I3" s="333"/>
+      <c r="J3" s="333"/>
+      <c r="K3" s="333"/>
+      <c r="L3" s="333"/>
+      <c r="M3" s="333"/>
+      <c r="N3" s="333"/>
+      <c r="O3" s="333"/>
+      <c r="P3" s="333"/>
+      <c r="Q3" s="333"/>
+      <c r="R3" s="333"/>
+      <c r="S3" s="333"/>
     </row>
     <row r="4" spans="1:26" s="232" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="326" t="s">
+      <c r="A4" s="334" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="327"/>
-      <c r="C4" s="327"/>
-      <c r="D4" s="327"/>
-      <c r="E4" s="327"/>
-      <c r="F4" s="327"/>
-      <c r="G4" s="327"/>
-      <c r="H4" s="327"/>
-      <c r="I4" s="327"/>
-      <c r="J4" s="327"/>
-      <c r="K4" s="327"/>
-      <c r="L4" s="327"/>
-      <c r="M4" s="327"/>
-      <c r="N4" s="327"/>
-      <c r="O4" s="327"/>
-      <c r="P4" s="327"/>
-      <c r="Q4" s="327"/>
-      <c r="R4" s="327"/>
-      <c r="S4" s="328"/>
+      <c r="B4" s="335"/>
+      <c r="C4" s="335"/>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="335"/>
+      <c r="H4" s="335"/>
+      <c r="I4" s="335"/>
+      <c r="J4" s="335"/>
+      <c r="K4" s="335"/>
+      <c r="L4" s="335"/>
+      <c r="M4" s="335"/>
+      <c r="N4" s="335"/>
+      <c r="O4" s="335"/>
+      <c r="P4" s="335"/>
+      <c r="Q4" s="335"/>
+      <c r="R4" s="335"/>
+      <c r="S4" s="336"/>
       <c r="U4" s="118"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -21917,58 +21904,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="234" customFormat="1">
-      <c r="A5" s="329" t="s">
+      <c r="A5" s="337" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="331" t="s">
+      <c r="B5" s="339" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="333" t="s">
+      <c r="C5" s="325" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="333" t="s">
+      <c r="D5" s="325" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="333" t="s">
+      <c r="E5" s="325" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="333" t="s">
+      <c r="F5" s="325" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="333" t="s">
+      <c r="G5" s="325" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="333" t="s">
+      <c r="H5" s="325" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="333" t="s">
+      <c r="I5" s="325" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="333" t="s">
+      <c r="J5" s="325" t="s">
         <v>125</v>
       </c>
-      <c r="K5" s="333" t="s">
+      <c r="K5" s="325" t="s">
         <v>126</v>
       </c>
-      <c r="L5" s="333" t="s">
+      <c r="L5" s="325" t="s">
         <v>127</v>
       </c>
-      <c r="M5" s="333" t="s">
+      <c r="M5" s="325" t="s">
         <v>128</v>
       </c>
-      <c r="N5" s="333" t="s">
+      <c r="N5" s="325" t="s">
         <v>129</v>
       </c>
-      <c r="O5" s="339" t="s">
+      <c r="O5" s="327" t="s">
         <v>130</v>
       </c>
-      <c r="P5" s="341" t="s">
+      <c r="P5" s="329" t="s">
         <v>131</v>
       </c>
-      <c r="Q5" s="337" t="s">
+      <c r="Q5" s="323" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="335" t="s">
+      <c r="R5" s="341" t="s">
         <v>132</v>
       </c>
       <c r="S5" s="233" t="s">
@@ -21981,24 +21968,24 @@
       <c r="Y5" s="236"/>
     </row>
     <row r="6" spans="1:26" s="234" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="330"/>
-      <c r="B6" s="332"/>
-      <c r="C6" s="334"/>
-      <c r="D6" s="334"/>
-      <c r="E6" s="334"/>
-      <c r="F6" s="334"/>
-      <c r="G6" s="334"/>
-      <c r="H6" s="334"/>
-      <c r="I6" s="334"/>
-      <c r="J6" s="334"/>
-      <c r="K6" s="334"/>
-      <c r="L6" s="334"/>
-      <c r="M6" s="334"/>
-      <c r="N6" s="334"/>
-      <c r="O6" s="340"/>
-      <c r="P6" s="342"/>
-      <c r="Q6" s="338"/>
-      <c r="R6" s="336"/>
+      <c r="A6" s="338"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="326"/>
+      <c r="D6" s="326"/>
+      <c r="E6" s="326"/>
+      <c r="F6" s="326"/>
+      <c r="G6" s="326"/>
+      <c r="H6" s="326"/>
+      <c r="I6" s="326"/>
+      <c r="J6" s="326"/>
+      <c r="K6" s="326"/>
+      <c r="L6" s="326"/>
+      <c r="M6" s="326"/>
+      <c r="N6" s="326"/>
+      <c r="O6" s="328"/>
+      <c r="P6" s="330"/>
+      <c r="Q6" s="324"/>
+      <c r="R6" s="342"/>
       <c r="S6" s="238" t="s">
         <v>133</v>
       </c>
@@ -22848,7 +22835,7 @@
     </row>
     <row r="26" spans="1:25" s="258" customFormat="1">
       <c r="A26" s="242" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B26" s="250">
         <v>1350</v>
@@ -22890,30 +22877,44 @@
     </row>
     <row r="27" spans="1:25" s="22" customFormat="1">
       <c r="A27" s="242" t="s">
-        <v>221</v>
-      </c>
-      <c r="B27" s="250"/>
-      <c r="C27" s="243"/>
-      <c r="D27" s="251"/>
+        <v>217</v>
+      </c>
+      <c r="B27" s="250">
+        <v>1500</v>
+      </c>
+      <c r="C27" s="243">
+        <v>450</v>
+      </c>
+      <c r="D27" s="251">
+        <v>20</v>
+      </c>
       <c r="E27" s="251"/>
       <c r="F27" s="251"/>
-      <c r="G27" s="251"/>
+      <c r="G27" s="251">
+        <v>280</v>
+      </c>
       <c r="H27" s="251"/>
       <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
+      <c r="J27" s="251">
+        <v>100</v>
+      </c>
+      <c r="K27" s="251">
+        <v>400</v>
+      </c>
       <c r="L27" s="251"/>
       <c r="M27" s="251">
         <v>1331</v>
       </c>
-      <c r="N27" s="285"/>
+      <c r="N27" s="285">
+        <v>20</v>
+      </c>
       <c r="O27" s="251"/>
       <c r="P27" s="251"/>
       <c r="Q27" s="251"/>
       <c r="R27" s="253"/>
       <c r="S27" s="247">
         <f t="shared" si="0"/>
-        <v>1331</v>
+        <v>4101</v>
       </c>
       <c r="T27" s="248"/>
       <c r="U27" s="7"/>
@@ -23184,15 +23185,15 @@
       </c>
       <c r="B38" s="268">
         <f>SUM(B7:B37)</f>
-        <v>18600</v>
+        <v>20100</v>
       </c>
       <c r="C38" s="269">
         <f t="shared" ref="C38:R38" si="1">SUM(C7:C37)</f>
-        <v>3580</v>
+        <v>4030</v>
       </c>
       <c r="D38" s="269">
         <f t="shared" si="1"/>
-        <v>665</v>
+        <v>685</v>
       </c>
       <c r="E38" s="269">
         <f t="shared" si="1"/>
@@ -23204,7 +23205,7 @@
       </c>
       <c r="G38" s="269">
         <f>SUM(G7:G37)</f>
-        <v>5090</v>
+        <v>5370</v>
       </c>
       <c r="H38" s="269">
         <f t="shared" si="1"/>
@@ -23216,11 +23217,11 @@
       </c>
       <c r="J38" s="269">
         <f t="shared" si="1"/>
-        <v>490</v>
+        <v>590</v>
       </c>
       <c r="K38" s="269">
         <f t="shared" si="1"/>
-        <v>9520</v>
+        <v>9920</v>
       </c>
       <c r="L38" s="269">
         <f t="shared" si="1"/>
@@ -23232,7 +23233,7 @@
       </c>
       <c r="N38" s="288">
         <f t="shared" si="1"/>
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="O38" s="269">
         <f t="shared" si="1"/>
@@ -23252,7 +23253,7 @@
       </c>
       <c r="S38" s="271">
         <f>SUM(S7:S37)</f>
-        <v>46451</v>
+        <v>49221</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -25257,12 +25258,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -25279,6 +25274,12 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>